<commit_message>
cahier + planning ok
</commit_message>
<xml_diff>
--- a/documentation/3_2_PlanningJeudiVendredi.xlsx
+++ b/documentation/3_2_PlanningJeudiVendredi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/theo_pasquier_studentfr_ch/Documents/3eme année/306/projet/306-G1-Piloter_un_robot_phidget_a_distance/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="548" documentId="8_{3242CAA9-CE1B-4AB7-A89C-0F9BBFF89D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{007E7C72-24A6-48FD-8C8E-3BB250EB8517}"/>
+  <xr:revisionPtr revIDLastSave="565" documentId="8_{3242CAA9-CE1B-4AB7-A89C-0F9BBFF89D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E452995-2E53-4286-95B3-DFAB6ED4D4BC}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -787,7 +787,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1316,6 +1316,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1369,8 +1381,8 @@
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
@@ -1388,7 +1400,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="5086350" y="685801"/>
-          <a:ext cx="4305301" cy="3990974"/>
+          <a:ext cx="4591050" cy="3990974"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -2011,7 +2023,7 @@
       <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AI32" sqref="AI32:AJ32"/>
+      <selection pane="bottomRight" activeCell="CA30" sqref="CA30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4122,15 +4134,15 @@
       <c r="AO22" s="59"/>
       <c r="AP22" s="59"/>
       <c r="AQ22" s="59"/>
-      <c r="AR22" s="60"/>
+      <c r="AR22" s="136"/>
       <c r="AS22" s="58"/>
       <c r="AT22" s="59"/>
       <c r="AU22" s="59"/>
       <c r="AV22" s="59"/>
       <c r="AW22" s="59"/>
-      <c r="AX22" s="59"/>
-      <c r="AY22" s="59"/>
-      <c r="AZ22" s="60"/>
+      <c r="AX22" s="135"/>
+      <c r="AY22" s="135"/>
+      <c r="AZ22" s="136"/>
       <c r="BA22" s="105"/>
       <c r="BB22" s="106"/>
       <c r="BC22" s="106"/>
@@ -4138,15 +4150,15 @@
       <c r="BE22" s="59"/>
       <c r="BF22" s="59"/>
       <c r="BG22" s="59"/>
-      <c r="BH22" s="60"/>
+      <c r="BH22" s="136"/>
       <c r="BI22" s="58"/>
       <c r="BJ22" s="59"/>
       <c r="BK22" s="59"/>
       <c r="BL22" s="59"/>
       <c r="BM22" s="59"/>
-      <c r="BN22" s="59"/>
-      <c r="BO22" s="59"/>
-      <c r="BP22" s="60"/>
+      <c r="BN22" s="135"/>
+      <c r="BO22" s="135"/>
+      <c r="BP22" s="136"/>
       <c r="BQ22" s="105"/>
       <c r="BR22" s="106"/>
       <c r="BS22" s="106"/>
@@ -4154,14 +4166,14 @@
       <c r="BU22" s="59"/>
       <c r="BV22" s="59"/>
       <c r="BW22" s="59"/>
-      <c r="BX22" s="60"/>
+      <c r="BX22" s="136"/>
       <c r="BY22" s="58"/>
       <c r="BZ22" s="59"/>
       <c r="CA22" s="59"/>
-      <c r="CB22" s="59"/>
-      <c r="CC22" s="59"/>
-      <c r="CD22" s="59"/>
-      <c r="CE22" s="59"/>
+      <c r="CB22" s="135"/>
+      <c r="CC22" s="135"/>
+      <c r="CD22" s="135"/>
+      <c r="CE22" s="135"/>
       <c r="CF22" s="60"/>
     </row>
     <row r="23" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4247,10 +4259,10 @@
       <c r="BY23" s="61"/>
       <c r="BZ23" s="62"/>
       <c r="CA23" s="62"/>
-      <c r="CB23" s="62"/>
-      <c r="CC23" s="62"/>
-      <c r="CD23" s="62"/>
-      <c r="CE23" s="62"/>
+      <c r="CB23" s="137"/>
+      <c r="CC23" s="137"/>
+      <c r="CD23" s="137"/>
+      <c r="CE23" s="137"/>
       <c r="CF23" s="63"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
planning + debut doc tâche
</commit_message>
<xml_diff>
--- a/documentation/3_2_PlanningJeudiVendredi.xlsx
+++ b/documentation/3_2_PlanningJeudiVendredi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/theo_pasquier_studentfr_ch/Documents/3eme année/306/projet/306-G1-Piloter_un_robot_phidget_a_distance/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="567" documentId="8_{3242CAA9-CE1B-4AB7-A89C-0F9BBFF89D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64637A20-91FE-4518-9853-634E9E5FED83}"/>
+  <xr:revisionPtr revIDLastSave="596" documentId="8_{3242CAA9-CE1B-4AB7-A89C-0F9BBFF89D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC739C07-F651-4C10-A8A9-8BB83FFCE789}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>Tâches</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Sprint review</t>
+  </si>
+  <si>
+    <t>En Cours</t>
   </si>
 </sst>
 </file>
@@ -1106,6 +1109,98 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1186,42 +1281,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1258,50 +1317,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1316,18 +1331,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1375,16 +1378,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1399,11 +1402,13 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5086350" y="657226"/>
-          <a:ext cx="4591050" cy="3990974"/>
+          <a:off x="5057775" y="676275"/>
+          <a:ext cx="5753100" cy="4010024"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj" fmla="val 17854"/>
+          </a:avLst>
         </a:prstGeom>
         <a:solidFill>
           <a:schemeClr val="accent6">
@@ -1429,63 +1434,6 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:endParaRPr lang="fr-CH" sz="900"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Losange 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE365392-7CEE-D70B-BE3F-0FC1177EECBF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9953625" y="2447925"/>
-          <a:ext cx="123825" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="diamond">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="fr-CH" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1632,6 +1580,63 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="16668750" y="3829050"/>
+          <a:ext cx="142875" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Losange 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C016B22A-05F8-4D01-860A-D3CF90744875}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10953750" y="2447925"/>
           <a:ext cx="142875" cy="209550"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
@@ -2023,7 +2028,7 @@
       <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AU32" sqref="AU32"/>
+      <selection pane="bottomRight" activeCell="AT27" sqref="AT27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2038,10 +2043,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:84" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="126"/>
+      <c r="B1" s="100"/>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
       <c r="E1" s="1"/>
@@ -2086,310 +2091,310 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="128"/>
+      <c r="B2" s="102"/>
       <c r="C2" s="13"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
-      <c r="K2" s="124"/>
-      <c r="L2" s="124"/>
-      <c r="M2" s="124"/>
-      <c r="N2" s="124"/>
-      <c r="O2" s="124"/>
-      <c r="P2" s="124"/>
-      <c r="Q2" s="124"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="124"/>
-      <c r="T2" s="124"/>
-      <c r="U2" s="124"/>
-      <c r="V2" s="124"/>
-      <c r="W2" s="124"/>
-      <c r="X2" s="124"/>
-      <c r="Y2" s="124"/>
-      <c r="Z2" s="124"/>
-      <c r="AA2" s="124"/>
-      <c r="AB2" s="124"/>
-      <c r="AC2" s="124"/>
-      <c r="AD2" s="124"/>
-      <c r="AE2" s="124"/>
-      <c r="AF2" s="124"/>
-      <c r="AG2" s="124"/>
-      <c r="AH2" s="124"/>
-      <c r="AI2" s="124"/>
-      <c r="AJ2" s="124"/>
-      <c r="AK2" s="124"/>
-      <c r="AL2" s="124"/>
-      <c r="AM2" s="124"/>
-      <c r="AN2" s="124"/>
-      <c r="AO2" s="124"/>
-      <c r="AP2" s="124"/>
-      <c r="AQ2" s="124"/>
-      <c r="AR2" s="124"/>
-      <c r="AS2" s="124"/>
-      <c r="AT2" s="124"/>
-      <c r="AU2" s="124"/>
-      <c r="AV2" s="124"/>
-      <c r="AW2" s="124"/>
-      <c r="AX2" s="124"/>
-      <c r="AY2" s="124"/>
-      <c r="AZ2" s="124"/>
-      <c r="BA2" s="124"/>
-      <c r="BB2" s="124"/>
-      <c r="BC2" s="124"/>
-      <c r="BD2" s="124"/>
-      <c r="BE2" s="124"/>
-      <c r="BF2" s="124"/>
-      <c r="BG2" s="124"/>
-      <c r="BH2" s="124"/>
-      <c r="BI2" s="124"/>
-      <c r="BJ2" s="124"/>
-      <c r="BK2" s="124"/>
-      <c r="BL2" s="124"/>
-      <c r="BM2" s="124"/>
-      <c r="BN2" s="124"/>
-      <c r="BO2" s="124"/>
-      <c r="BP2" s="124"/>
-      <c r="BQ2" s="124"/>
-      <c r="BR2" s="124"/>
-      <c r="BS2" s="124"/>
-      <c r="BT2" s="124"/>
-      <c r="BU2" s="124"/>
-      <c r="BV2" s="124"/>
-      <c r="BW2" s="124"/>
-      <c r="BX2" s="124"/>
-      <c r="BY2" s="124"/>
-      <c r="BZ2" s="124"/>
-      <c r="CA2" s="124"/>
-      <c r="CB2" s="124"/>
-      <c r="CC2" s="124"/>
-      <c r="CD2" s="124"/>
-      <c r="CE2" s="124"/>
-      <c r="CF2" s="124"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
+      <c r="V2" s="98"/>
+      <c r="W2" s="98"/>
+      <c r="X2" s="98"/>
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="98"/>
+      <c r="AA2" s="98"/>
+      <c r="AB2" s="98"/>
+      <c r="AC2" s="98"/>
+      <c r="AD2" s="98"/>
+      <c r="AE2" s="98"/>
+      <c r="AF2" s="98"/>
+      <c r="AG2" s="98"/>
+      <c r="AH2" s="98"/>
+      <c r="AI2" s="98"/>
+      <c r="AJ2" s="98"/>
+      <c r="AK2" s="98"/>
+      <c r="AL2" s="98"/>
+      <c r="AM2" s="98"/>
+      <c r="AN2" s="98"/>
+      <c r="AO2" s="98"/>
+      <c r="AP2" s="98"/>
+      <c r="AQ2" s="98"/>
+      <c r="AR2" s="98"/>
+      <c r="AS2" s="98"/>
+      <c r="AT2" s="98"/>
+      <c r="AU2" s="98"/>
+      <c r="AV2" s="98"/>
+      <c r="AW2" s="98"/>
+      <c r="AX2" s="98"/>
+      <c r="AY2" s="98"/>
+      <c r="AZ2" s="98"/>
+      <c r="BA2" s="98"/>
+      <c r="BB2" s="98"/>
+      <c r="BC2" s="98"/>
+      <c r="BD2" s="98"/>
+      <c r="BE2" s="98"/>
+      <c r="BF2" s="98"/>
+      <c r="BG2" s="98"/>
+      <c r="BH2" s="98"/>
+      <c r="BI2" s="98"/>
+      <c r="BJ2" s="98"/>
+      <c r="BK2" s="98"/>
+      <c r="BL2" s="98"/>
+      <c r="BM2" s="98"/>
+      <c r="BN2" s="98"/>
+      <c r="BO2" s="98"/>
+      <c r="BP2" s="98"/>
+      <c r="BQ2" s="98"/>
+      <c r="BR2" s="98"/>
+      <c r="BS2" s="98"/>
+      <c r="BT2" s="98"/>
+      <c r="BU2" s="98"/>
+      <c r="BV2" s="98"/>
+      <c r="BW2" s="98"/>
+      <c r="BX2" s="98"/>
+      <c r="BY2" s="98"/>
+      <c r="BZ2" s="98"/>
+      <c r="CA2" s="98"/>
+      <c r="CB2" s="98"/>
+      <c r="CC2" s="98"/>
+      <c r="CD2" s="98"/>
+      <c r="CE2" s="98"/>
+      <c r="CF2" s="98"/>
     </row>
     <row r="3" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="125"/>
-      <c r="F3" s="125"/>
-      <c r="G3" s="125"/>
-      <c r="H3" s="125"/>
-      <c r="I3" s="125"/>
-      <c r="J3" s="125"/>
-      <c r="K3" s="125"/>
-      <c r="L3" s="125"/>
-      <c r="M3" s="125"/>
-      <c r="N3" s="125"/>
-      <c r="O3" s="125"/>
-      <c r="P3" s="125"/>
-      <c r="Q3" s="125"/>
-      <c r="R3" s="125"/>
-      <c r="S3" s="125"/>
-      <c r="T3" s="125"/>
-      <c r="U3" s="125"/>
-      <c r="V3" s="125"/>
-      <c r="W3" s="125"/>
-      <c r="X3" s="125"/>
-      <c r="Y3" s="125"/>
-      <c r="Z3" s="125"/>
-      <c r="AA3" s="125"/>
-      <c r="AB3" s="125"/>
-      <c r="AC3" s="125"/>
-      <c r="AD3" s="125"/>
-      <c r="AE3" s="125"/>
-      <c r="AF3" s="125"/>
-      <c r="AG3" s="125"/>
-      <c r="AH3" s="125"/>
-      <c r="AI3" s="125"/>
-      <c r="AJ3" s="125"/>
-      <c r="AK3" s="125"/>
-      <c r="AL3" s="125"/>
-      <c r="AM3" s="125"/>
-      <c r="AN3" s="125"/>
-      <c r="AO3" s="125"/>
-      <c r="AP3" s="125"/>
-      <c r="AQ3" s="125"/>
-      <c r="AR3" s="125"/>
-      <c r="AS3" s="125"/>
-      <c r="AT3" s="125"/>
-      <c r="AU3" s="125"/>
-      <c r="AV3" s="125"/>
-      <c r="AW3" s="125"/>
-      <c r="AX3" s="125"/>
-      <c r="AY3" s="125"/>
-      <c r="AZ3" s="125"/>
-      <c r="BA3" s="125"/>
-      <c r="BB3" s="125"/>
-      <c r="BC3" s="125"/>
-      <c r="BD3" s="125"/>
-      <c r="BE3" s="125"/>
-      <c r="BF3" s="125"/>
-      <c r="BG3" s="125"/>
-      <c r="BH3" s="125"/>
-      <c r="BI3" s="125"/>
-      <c r="BJ3" s="125"/>
-      <c r="BK3" s="125"/>
-      <c r="BL3" s="125"/>
-      <c r="BM3" s="125"/>
-      <c r="BN3" s="125"/>
-      <c r="BO3" s="125"/>
-      <c r="BP3" s="125"/>
-      <c r="BQ3" s="125"/>
-      <c r="BR3" s="125"/>
-      <c r="BS3" s="125"/>
-      <c r="BT3" s="125"/>
-      <c r="BU3" s="125"/>
-      <c r="BV3" s="125"/>
-      <c r="BW3" s="125"/>
-      <c r="BX3" s="125"/>
-      <c r="BY3" s="125"/>
-      <c r="BZ3" s="125"/>
-      <c r="CA3" s="125"/>
-      <c r="CB3" s="125"/>
-      <c r="CC3" s="125"/>
-      <c r="CD3" s="125"/>
-      <c r="CE3" s="125"/>
-      <c r="CF3" s="125"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
+      <c r="Q3" s="99"/>
+      <c r="R3" s="99"/>
+      <c r="S3" s="99"/>
+      <c r="T3" s="99"/>
+      <c r="U3" s="99"/>
+      <c r="V3" s="99"/>
+      <c r="W3" s="99"/>
+      <c r="X3" s="99"/>
+      <c r="Y3" s="99"/>
+      <c r="Z3" s="99"/>
+      <c r="AA3" s="99"/>
+      <c r="AB3" s="99"/>
+      <c r="AC3" s="99"/>
+      <c r="AD3" s="99"/>
+      <c r="AE3" s="99"/>
+      <c r="AF3" s="99"/>
+      <c r="AG3" s="99"/>
+      <c r="AH3" s="99"/>
+      <c r="AI3" s="99"/>
+      <c r="AJ3" s="99"/>
+      <c r="AK3" s="99"/>
+      <c r="AL3" s="99"/>
+      <c r="AM3" s="99"/>
+      <c r="AN3" s="99"/>
+      <c r="AO3" s="99"/>
+      <c r="AP3" s="99"/>
+      <c r="AQ3" s="99"/>
+      <c r="AR3" s="99"/>
+      <c r="AS3" s="99"/>
+      <c r="AT3" s="99"/>
+      <c r="AU3" s="99"/>
+      <c r="AV3" s="99"/>
+      <c r="AW3" s="99"/>
+      <c r="AX3" s="99"/>
+      <c r="AY3" s="99"/>
+      <c r="AZ3" s="99"/>
+      <c r="BA3" s="99"/>
+      <c r="BB3" s="99"/>
+      <c r="BC3" s="99"/>
+      <c r="BD3" s="99"/>
+      <c r="BE3" s="99"/>
+      <c r="BF3" s="99"/>
+      <c r="BG3" s="99"/>
+      <c r="BH3" s="99"/>
+      <c r="BI3" s="99"/>
+      <c r="BJ3" s="99"/>
+      <c r="BK3" s="99"/>
+      <c r="BL3" s="99"/>
+      <c r="BM3" s="99"/>
+      <c r="BN3" s="99"/>
+      <c r="BO3" s="99"/>
+      <c r="BP3" s="99"/>
+      <c r="BQ3" s="99"/>
+      <c r="BR3" s="99"/>
+      <c r="BS3" s="99"/>
+      <c r="BT3" s="99"/>
+      <c r="BU3" s="99"/>
+      <c r="BV3" s="99"/>
+      <c r="BW3" s="99"/>
+      <c r="BX3" s="99"/>
+      <c r="BY3" s="99"/>
+      <c r="BZ3" s="99"/>
+      <c r="CA3" s="99"/>
+      <c r="CB3" s="99"/>
+      <c r="CC3" s="99"/>
+      <c r="CD3" s="99"/>
+      <c r="CE3" s="99"/>
+      <c r="CF3" s="99"/>
     </row>
     <row r="4" spans="1:84" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="129" t="s">
+      <c r="A4" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="130"/>
+      <c r="B4" s="104"/>
       <c r="C4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="120" t="s">
+      <c r="E4" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="121"/>
-      <c r="I4" s="122">
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="85">
         <v>45995</v>
       </c>
-      <c r="J4" s="122"/>
-      <c r="K4" s="122"/>
-      <c r="L4" s="123"/>
-      <c r="M4" s="120" t="s">
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="121"/>
-      <c r="O4" s="121"/>
-      <c r="P4" s="121"/>
-      <c r="Q4" s="122">
+      <c r="N4" s="88"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="85">
         <v>45996</v>
       </c>
-      <c r="R4" s="122"/>
-      <c r="S4" s="122"/>
-      <c r="T4" s="123"/>
-      <c r="U4" s="120" t="s">
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="121"/>
-      <c r="W4" s="121"/>
-      <c r="X4" s="121"/>
-      <c r="Y4" s="122">
+      <c r="V4" s="88"/>
+      <c r="W4" s="88"/>
+      <c r="X4" s="88"/>
+      <c r="Y4" s="85">
         <v>46002</v>
       </c>
-      <c r="Z4" s="122"/>
-      <c r="AA4" s="122"/>
-      <c r="AB4" s="123"/>
-      <c r="AC4" s="120" t="s">
+      <c r="Z4" s="85"/>
+      <c r="AA4" s="85"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="121"/>
-      <c r="AE4" s="121"/>
-      <c r="AF4" s="121"/>
-      <c r="AG4" s="122">
+      <c r="AD4" s="88"/>
+      <c r="AE4" s="88"/>
+      <c r="AF4" s="88"/>
+      <c r="AG4" s="85">
         <v>46003</v>
       </c>
-      <c r="AH4" s="122"/>
-      <c r="AI4" s="122"/>
-      <c r="AJ4" s="123"/>
-      <c r="AK4" s="120" t="s">
+      <c r="AH4" s="85"/>
+      <c r="AI4" s="85"/>
+      <c r="AJ4" s="86"/>
+      <c r="AK4" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="AL4" s="121"/>
-      <c r="AM4" s="121"/>
-      <c r="AN4" s="121"/>
-      <c r="AO4" s="122">
+      <c r="AL4" s="88"/>
+      <c r="AM4" s="88"/>
+      <c r="AN4" s="88"/>
+      <c r="AO4" s="85">
         <v>46009</v>
       </c>
-      <c r="AP4" s="122"/>
-      <c r="AQ4" s="122"/>
-      <c r="AR4" s="123"/>
-      <c r="AS4" s="120" t="s">
+      <c r="AP4" s="85"/>
+      <c r="AQ4" s="85"/>
+      <c r="AR4" s="86"/>
+      <c r="AS4" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="AT4" s="121"/>
-      <c r="AU4" s="121"/>
-      <c r="AV4" s="121"/>
-      <c r="AW4" s="122">
+      <c r="AT4" s="88"/>
+      <c r="AU4" s="88"/>
+      <c r="AV4" s="88"/>
+      <c r="AW4" s="85">
         <v>46010</v>
       </c>
-      <c r="AX4" s="122"/>
-      <c r="AY4" s="122"/>
-      <c r="AZ4" s="123"/>
-      <c r="BA4" s="120" t="s">
+      <c r="AX4" s="85"/>
+      <c r="AY4" s="85"/>
+      <c r="AZ4" s="86"/>
+      <c r="BA4" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="BB4" s="121"/>
-      <c r="BC4" s="121"/>
-      <c r="BD4" s="121"/>
-      <c r="BE4" s="122">
+      <c r="BB4" s="88"/>
+      <c r="BC4" s="88"/>
+      <c r="BD4" s="88"/>
+      <c r="BE4" s="85">
         <v>46030</v>
       </c>
-      <c r="BF4" s="122"/>
-      <c r="BG4" s="122"/>
-      <c r="BH4" s="123"/>
-      <c r="BI4" s="120" t="s">
+      <c r="BF4" s="85"/>
+      <c r="BG4" s="85"/>
+      <c r="BH4" s="86"/>
+      <c r="BI4" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="BJ4" s="121"/>
-      <c r="BK4" s="121"/>
-      <c r="BL4" s="121"/>
-      <c r="BM4" s="122">
+      <c r="BJ4" s="88"/>
+      <c r="BK4" s="88"/>
+      <c r="BL4" s="88"/>
+      <c r="BM4" s="85">
         <v>46031</v>
       </c>
-      <c r="BN4" s="122"/>
-      <c r="BO4" s="122"/>
-      <c r="BP4" s="123"/>
-      <c r="BQ4" s="120" t="s">
+      <c r="BN4" s="85"/>
+      <c r="BO4" s="85"/>
+      <c r="BP4" s="86"/>
+      <c r="BQ4" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="BR4" s="121"/>
-      <c r="BS4" s="121"/>
-      <c r="BT4" s="121"/>
-      <c r="BU4" s="122">
+      <c r="BR4" s="88"/>
+      <c r="BS4" s="88"/>
+      <c r="BT4" s="88"/>
+      <c r="BU4" s="85">
         <v>46037</v>
       </c>
-      <c r="BV4" s="122"/>
-      <c r="BW4" s="122"/>
-      <c r="BX4" s="123"/>
-      <c r="BY4" s="120" t="s">
+      <c r="BV4" s="85"/>
+      <c r="BW4" s="85"/>
+      <c r="BX4" s="86"/>
+      <c r="BY4" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="BZ4" s="121"/>
-      <c r="CA4" s="121"/>
-      <c r="CB4" s="121"/>
-      <c r="CC4" s="122">
+      <c r="BZ4" s="88"/>
+      <c r="CA4" s="88"/>
+      <c r="CB4" s="88"/>
+      <c r="CC4" s="85">
         <v>46038</v>
       </c>
-      <c r="CD4" s="122"/>
-      <c r="CE4" s="122"/>
-      <c r="CF4" s="123"/>
+      <c r="CD4" s="85"/>
+      <c r="CE4" s="85"/>
+      <c r="CF4" s="86"/>
     </row>
     <row r="5" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="129"/>
-      <c r="B5" s="130"/>
+      <c r="A5" s="103"/>
+      <c r="B5" s="104"/>
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
@@ -2638,7 +2643,7 @@
       </c>
     </row>
     <row r="6" spans="1:84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="131" t="s">
+      <c r="A6" s="134" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="27" t="s">
@@ -2648,12 +2653,12 @@
         <v>23</v>
       </c>
       <c r="D6" s="24"/>
-      <c r="E6" s="84" t="s">
+      <c r="E6" s="107" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="86"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="109"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="17"/>
@@ -2666,16 +2671,16 @@
       <c r="R6" s="30"/>
       <c r="S6" s="30"/>
       <c r="T6" s="31"/>
-      <c r="U6" s="93" t="s">
+      <c r="U6" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="V6" s="94"/>
-      <c r="W6" s="94"/>
-      <c r="X6" s="94"/>
-      <c r="Y6" s="94"/>
-      <c r="Z6" s="94"/>
-      <c r="AA6" s="94"/>
-      <c r="AB6" s="95"/>
+      <c r="V6" s="117"/>
+      <c r="W6" s="117"/>
+      <c r="X6" s="117"/>
+      <c r="Y6" s="117"/>
+      <c r="Z6" s="117"/>
+      <c r="AA6" s="117"/>
+      <c r="AB6" s="118"/>
       <c r="AC6" s="32"/>
       <c r="AD6" s="30"/>
       <c r="AE6" s="30"/>
@@ -2684,12 +2689,12 @@
       <c r="AH6" s="30"/>
       <c r="AI6" s="30"/>
       <c r="AJ6" s="31"/>
-      <c r="AK6" s="102" t="s">
+      <c r="AK6" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="AL6" s="103"/>
-      <c r="AM6" s="103"/>
-      <c r="AN6" s="104"/>
+      <c r="AL6" s="90"/>
+      <c r="AM6" s="90"/>
+      <c r="AN6" s="91"/>
       <c r="AO6" s="30"/>
       <c r="AP6" s="30"/>
       <c r="AQ6" s="30"/>
@@ -2702,12 +2707,12 @@
       <c r="AX6" s="30"/>
       <c r="AY6" s="30"/>
       <c r="AZ6" s="31"/>
-      <c r="BA6" s="102" t="s">
+      <c r="BA6" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="BB6" s="103"/>
-      <c r="BC6" s="103"/>
-      <c r="BD6" s="104"/>
+      <c r="BB6" s="90"/>
+      <c r="BC6" s="90"/>
+      <c r="BD6" s="91"/>
       <c r="BE6" s="30"/>
       <c r="BF6" s="30"/>
       <c r="BG6" s="30"/>
@@ -2720,12 +2725,12 @@
       <c r="BN6" s="30"/>
       <c r="BO6" s="30"/>
       <c r="BP6" s="31"/>
-      <c r="BQ6" s="102" t="s">
+      <c r="BQ6" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="BR6" s="103"/>
-      <c r="BS6" s="103"/>
-      <c r="BT6" s="104"/>
+      <c r="BR6" s="90"/>
+      <c r="BS6" s="90"/>
+      <c r="BT6" s="91"/>
       <c r="BU6" s="71"/>
       <c r="BV6" s="71"/>
       <c r="BW6" s="30"/>
@@ -2740,7 +2745,7 @@
       <c r="CF6" s="31"/>
     </row>
     <row r="7" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A7" s="131"/>
+      <c r="A7" s="134"/>
       <c r="B7" s="28" t="s">
         <v>11</v>
       </c>
@@ -2748,10 +2753,10 @@
         <v>23</v>
       </c>
       <c r="D7" s="25"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="89"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="112"/>
       <c r="I7" s="33"/>
       <c r="J7" s="33"/>
       <c r="K7" s="33"/>
@@ -2764,14 +2769,14 @@
       <c r="R7" s="33"/>
       <c r="S7" s="33"/>
       <c r="T7" s="34"/>
-      <c r="U7" s="96"/>
-      <c r="V7" s="97"/>
-      <c r="W7" s="97"/>
-      <c r="X7" s="97"/>
-      <c r="Y7" s="97"/>
-      <c r="Z7" s="97"/>
-      <c r="AA7" s="97"/>
-      <c r="AB7" s="98"/>
+      <c r="U7" s="119"/>
+      <c r="V7" s="120"/>
+      <c r="W7" s="120"/>
+      <c r="X7" s="120"/>
+      <c r="Y7" s="120"/>
+      <c r="Z7" s="120"/>
+      <c r="AA7" s="120"/>
+      <c r="AB7" s="121"/>
       <c r="AC7" s="35"/>
       <c r="AD7" s="33"/>
       <c r="AE7" s="33"/>
@@ -2780,10 +2785,10 @@
       <c r="AH7" s="33"/>
       <c r="AI7" s="33"/>
       <c r="AJ7" s="34"/>
-      <c r="AK7" s="105"/>
-      <c r="AL7" s="106"/>
-      <c r="AM7" s="106"/>
-      <c r="AN7" s="107"/>
+      <c r="AK7" s="92"/>
+      <c r="AL7" s="93"/>
+      <c r="AM7" s="93"/>
+      <c r="AN7" s="94"/>
       <c r="AO7" s="33"/>
       <c r="AP7" s="33"/>
       <c r="AQ7" s="33"/>
@@ -2796,10 +2801,10 @@
       <c r="AX7" s="33"/>
       <c r="AY7" s="33"/>
       <c r="AZ7" s="34"/>
-      <c r="BA7" s="105"/>
-      <c r="BB7" s="106"/>
-      <c r="BC7" s="106"/>
-      <c r="BD7" s="107"/>
+      <c r="BA7" s="92"/>
+      <c r="BB7" s="93"/>
+      <c r="BC7" s="93"/>
+      <c r="BD7" s="94"/>
       <c r="BE7" s="33"/>
       <c r="BF7" s="33"/>
       <c r="BG7" s="33"/>
@@ -2812,10 +2817,10 @@
       <c r="BN7" s="33"/>
       <c r="BO7" s="33"/>
       <c r="BP7" s="34"/>
-      <c r="BQ7" s="105"/>
-      <c r="BR7" s="106"/>
-      <c r="BS7" s="106"/>
-      <c r="BT7" s="107"/>
+      <c r="BQ7" s="92"/>
+      <c r="BR7" s="93"/>
+      <c r="BS7" s="93"/>
+      <c r="BT7" s="94"/>
       <c r="BU7" s="33"/>
       <c r="BV7" s="33"/>
       <c r="BW7" s="33"/>
@@ -2830,7 +2835,7 @@
       <c r="CF7" s="34"/>
     </row>
     <row r="8" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A8" s="131"/>
+      <c r="A8" s="134"/>
       <c r="B8" s="29" t="s">
         <v>12</v>
       </c>
@@ -2838,10 +2843,10 @@
         <v>23</v>
       </c>
       <c r="D8" s="25"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="88"/>
-      <c r="H8" s="89"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="112"/>
       <c r="I8" s="33"/>
       <c r="J8" s="33"/>
       <c r="K8" s="33"/>
@@ -2854,14 +2859,14 @@
       <c r="R8" s="33"/>
       <c r="S8" s="33"/>
       <c r="T8" s="34"/>
-      <c r="U8" s="96"/>
-      <c r="V8" s="97"/>
-      <c r="W8" s="97"/>
-      <c r="X8" s="97"/>
-      <c r="Y8" s="97"/>
-      <c r="Z8" s="97"/>
-      <c r="AA8" s="97"/>
-      <c r="AB8" s="98"/>
+      <c r="U8" s="119"/>
+      <c r="V8" s="120"/>
+      <c r="W8" s="120"/>
+      <c r="X8" s="120"/>
+      <c r="Y8" s="120"/>
+      <c r="Z8" s="120"/>
+      <c r="AA8" s="120"/>
+      <c r="AB8" s="121"/>
       <c r="AC8" s="35"/>
       <c r="AD8" s="33"/>
       <c r="AE8" s="33"/>
@@ -2870,10 +2875,10 @@
       <c r="AH8" s="33"/>
       <c r="AI8" s="33"/>
       <c r="AJ8" s="34"/>
-      <c r="AK8" s="105"/>
-      <c r="AL8" s="106"/>
-      <c r="AM8" s="106"/>
-      <c r="AN8" s="107"/>
+      <c r="AK8" s="92"/>
+      <c r="AL8" s="93"/>
+      <c r="AM8" s="93"/>
+      <c r="AN8" s="94"/>
       <c r="AO8" s="33"/>
       <c r="AP8" s="33"/>
       <c r="AQ8" s="33"/>
@@ -2886,10 +2891,10 @@
       <c r="AX8" s="33"/>
       <c r="AY8" s="33"/>
       <c r="AZ8" s="34"/>
-      <c r="BA8" s="105"/>
-      <c r="BB8" s="106"/>
-      <c r="BC8" s="106"/>
-      <c r="BD8" s="107"/>
+      <c r="BA8" s="92"/>
+      <c r="BB8" s="93"/>
+      <c r="BC8" s="93"/>
+      <c r="BD8" s="94"/>
       <c r="BE8" s="33"/>
       <c r="BF8" s="33"/>
       <c r="BG8" s="33"/>
@@ -2902,10 +2907,10 @@
       <c r="BN8" s="33"/>
       <c r="BO8" s="33"/>
       <c r="BP8" s="34"/>
-      <c r="BQ8" s="105"/>
-      <c r="BR8" s="106"/>
-      <c r="BS8" s="106"/>
-      <c r="BT8" s="107"/>
+      <c r="BQ8" s="92"/>
+      <c r="BR8" s="93"/>
+      <c r="BS8" s="93"/>
+      <c r="BT8" s="94"/>
       <c r="BU8" s="33"/>
       <c r="BV8" s="33"/>
       <c r="BW8" s="33"/>
@@ -2920,7 +2925,7 @@
       <c r="CF8" s="34"/>
     </row>
     <row r="9" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A9" s="132" t="s">
+      <c r="A9" s="135" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="36" t="s">
@@ -2930,10 +2935,10 @@
         <v>23</v>
       </c>
       <c r="D9" s="25"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="88"/>
-      <c r="H9" s="89"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="112"/>
       <c r="I9" s="37"/>
       <c r="J9" s="37"/>
       <c r="K9" s="37"/>
@@ -2946,14 +2951,14 @@
       <c r="R9" s="20"/>
       <c r="S9" s="20"/>
       <c r="T9" s="38"/>
-      <c r="U9" s="96"/>
-      <c r="V9" s="97"/>
-      <c r="W9" s="97"/>
-      <c r="X9" s="97"/>
-      <c r="Y9" s="97"/>
-      <c r="Z9" s="97"/>
-      <c r="AA9" s="97"/>
-      <c r="AB9" s="98"/>
+      <c r="U9" s="119"/>
+      <c r="V9" s="120"/>
+      <c r="W9" s="120"/>
+      <c r="X9" s="120"/>
+      <c r="Y9" s="120"/>
+      <c r="Z9" s="120"/>
+      <c r="AA9" s="120"/>
+      <c r="AB9" s="121"/>
       <c r="AC9" s="39"/>
       <c r="AD9" s="37"/>
       <c r="AE9" s="37"/>
@@ -2962,10 +2967,10 @@
       <c r="AH9" s="37"/>
       <c r="AI9" s="37"/>
       <c r="AJ9" s="38"/>
-      <c r="AK9" s="105"/>
-      <c r="AL9" s="106"/>
-      <c r="AM9" s="106"/>
-      <c r="AN9" s="107"/>
+      <c r="AK9" s="92"/>
+      <c r="AL9" s="93"/>
+      <c r="AM9" s="93"/>
+      <c r="AN9" s="94"/>
       <c r="AO9" s="37"/>
       <c r="AP9" s="37"/>
       <c r="AQ9" s="37"/>
@@ -2978,10 +2983,10 @@
       <c r="AX9" s="37"/>
       <c r="AY9" s="37"/>
       <c r="AZ9" s="38"/>
-      <c r="BA9" s="105"/>
-      <c r="BB9" s="106"/>
-      <c r="BC9" s="106"/>
-      <c r="BD9" s="107"/>
+      <c r="BA9" s="92"/>
+      <c r="BB9" s="93"/>
+      <c r="BC9" s="93"/>
+      <c r="BD9" s="94"/>
       <c r="BE9" s="37"/>
       <c r="BF9" s="37"/>
       <c r="BG9" s="37"/>
@@ -2994,10 +2999,10 @@
       <c r="BN9" s="37"/>
       <c r="BO9" s="37"/>
       <c r="BP9" s="38"/>
-      <c r="BQ9" s="105"/>
-      <c r="BR9" s="106"/>
-      <c r="BS9" s="106"/>
-      <c r="BT9" s="107"/>
+      <c r="BQ9" s="92"/>
+      <c r="BR9" s="93"/>
+      <c r="BS9" s="93"/>
+      <c r="BT9" s="94"/>
       <c r="BU9" s="37"/>
       <c r="BV9" s="37"/>
       <c r="BW9" s="37"/>
@@ -3012,7 +3017,7 @@
       <c r="CF9" s="38"/>
     </row>
     <row r="10" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A10" s="133"/>
+      <c r="A10" s="136"/>
       <c r="B10" s="36" t="s">
         <v>15</v>
       </c>
@@ -3020,10 +3025,10 @@
         <v>23</v>
       </c>
       <c r="D10" s="25"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="89"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="112"/>
       <c r="I10" s="37"/>
       <c r="J10" s="37"/>
       <c r="K10" s="37"/>
@@ -3036,14 +3041,14 @@
       <c r="R10" s="20"/>
       <c r="S10" s="20"/>
       <c r="T10" s="38"/>
-      <c r="U10" s="96"/>
-      <c r="V10" s="97"/>
-      <c r="W10" s="97"/>
-      <c r="X10" s="97"/>
-      <c r="Y10" s="97"/>
-      <c r="Z10" s="97"/>
-      <c r="AA10" s="97"/>
-      <c r="AB10" s="98"/>
+      <c r="U10" s="119"/>
+      <c r="V10" s="120"/>
+      <c r="W10" s="120"/>
+      <c r="X10" s="120"/>
+      <c r="Y10" s="120"/>
+      <c r="Z10" s="120"/>
+      <c r="AA10" s="120"/>
+      <c r="AB10" s="121"/>
       <c r="AC10" s="39"/>
       <c r="AD10" s="37"/>
       <c r="AE10" s="37"/>
@@ -3052,10 +3057,10 @@
       <c r="AH10" s="37"/>
       <c r="AI10" s="37"/>
       <c r="AJ10" s="38"/>
-      <c r="AK10" s="105"/>
-      <c r="AL10" s="106"/>
-      <c r="AM10" s="106"/>
-      <c r="AN10" s="107"/>
+      <c r="AK10" s="92"/>
+      <c r="AL10" s="93"/>
+      <c r="AM10" s="93"/>
+      <c r="AN10" s="94"/>
       <c r="AO10" s="37"/>
       <c r="AP10" s="37"/>
       <c r="AQ10" s="37"/>
@@ -3068,10 +3073,10 @@
       <c r="AX10" s="37"/>
       <c r="AY10" s="37"/>
       <c r="AZ10" s="38"/>
-      <c r="BA10" s="105"/>
-      <c r="BB10" s="106"/>
-      <c r="BC10" s="106"/>
-      <c r="BD10" s="107"/>
+      <c r="BA10" s="92"/>
+      <c r="BB10" s="93"/>
+      <c r="BC10" s="93"/>
+      <c r="BD10" s="94"/>
       <c r="BE10" s="37"/>
       <c r="BF10" s="37"/>
       <c r="BG10" s="37"/>
@@ -3084,10 +3089,10 @@
       <c r="BN10" s="37"/>
       <c r="BO10" s="37"/>
       <c r="BP10" s="38"/>
-      <c r="BQ10" s="105"/>
-      <c r="BR10" s="106"/>
-      <c r="BS10" s="106"/>
-      <c r="BT10" s="107"/>
+      <c r="BQ10" s="92"/>
+      <c r="BR10" s="93"/>
+      <c r="BS10" s="93"/>
+      <c r="BT10" s="94"/>
       <c r="BU10" s="37"/>
       <c r="BV10" s="37"/>
       <c r="BW10" s="37"/>
@@ -3102,7 +3107,7 @@
       <c r="CF10" s="38"/>
     </row>
     <row r="11" spans="1:84" x14ac:dyDescent="0.2">
-      <c r="A11" s="134"/>
+      <c r="A11" s="137"/>
       <c r="B11" s="36" t="s">
         <v>16</v>
       </c>
@@ -3110,10 +3115,10 @@
         <v>23</v>
       </c>
       <c r="D11" s="25"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="89"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="112"/>
       <c r="I11" s="37"/>
       <c r="J11" s="37"/>
       <c r="K11" s="37"/>
@@ -3126,14 +3131,14 @@
       <c r="R11" s="37"/>
       <c r="S11" s="37"/>
       <c r="T11" s="21"/>
-      <c r="U11" s="96"/>
-      <c r="V11" s="97"/>
-      <c r="W11" s="97"/>
-      <c r="X11" s="97"/>
-      <c r="Y11" s="97"/>
-      <c r="Z11" s="97"/>
-      <c r="AA11" s="97"/>
-      <c r="AB11" s="98"/>
+      <c r="U11" s="119"/>
+      <c r="V11" s="120"/>
+      <c r="W11" s="120"/>
+      <c r="X11" s="120"/>
+      <c r="Y11" s="120"/>
+      <c r="Z11" s="120"/>
+      <c r="AA11" s="120"/>
+      <c r="AB11" s="121"/>
       <c r="AC11" s="22"/>
       <c r="AD11" s="37"/>
       <c r="AE11" s="37"/>
@@ -3142,10 +3147,10 @@
       <c r="AH11" s="37"/>
       <c r="AI11" s="37"/>
       <c r="AJ11" s="38"/>
-      <c r="AK11" s="105"/>
-      <c r="AL11" s="106"/>
-      <c r="AM11" s="106"/>
-      <c r="AN11" s="107"/>
+      <c r="AK11" s="92"/>
+      <c r="AL11" s="93"/>
+      <c r="AM11" s="93"/>
+      <c r="AN11" s="94"/>
       <c r="AO11" s="37"/>
       <c r="AP11" s="37"/>
       <c r="AQ11" s="37"/>
@@ -3158,10 +3163,10 @@
       <c r="AX11" s="37"/>
       <c r="AY11" s="37"/>
       <c r="AZ11" s="38"/>
-      <c r="BA11" s="105"/>
-      <c r="BB11" s="106"/>
-      <c r="BC11" s="106"/>
-      <c r="BD11" s="107"/>
+      <c r="BA11" s="92"/>
+      <c r="BB11" s="93"/>
+      <c r="BC11" s="93"/>
+      <c r="BD11" s="94"/>
       <c r="BE11" s="37"/>
       <c r="BF11" s="37"/>
       <c r="BG11" s="37"/>
@@ -3174,10 +3179,10 @@
       <c r="BN11" s="37"/>
       <c r="BO11" s="37"/>
       <c r="BP11" s="38"/>
-      <c r="BQ11" s="105"/>
-      <c r="BR11" s="106"/>
-      <c r="BS11" s="106"/>
-      <c r="BT11" s="107"/>
+      <c r="BQ11" s="92"/>
+      <c r="BR11" s="93"/>
+      <c r="BS11" s="93"/>
+      <c r="BT11" s="94"/>
       <c r="BU11" s="37"/>
       <c r="BV11" s="37"/>
       <c r="BW11" s="37"/>
@@ -3192,7 +3197,7 @@
       <c r="CF11" s="38"/>
     </row>
     <row r="12" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="115" t="s">
+      <c r="A12" s="129" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="74" t="s">
@@ -3202,10 +3207,10 @@
         <v>24</v>
       </c>
       <c r="D12" s="25"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="89"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="112"/>
       <c r="I12" s="40"/>
       <c r="J12" s="40"/>
       <c r="K12" s="40"/>
@@ -3218,14 +3223,14 @@
       <c r="R12" s="40"/>
       <c r="S12" s="40"/>
       <c r="T12" s="41"/>
-      <c r="U12" s="96"/>
-      <c r="V12" s="97"/>
-      <c r="W12" s="97"/>
-      <c r="X12" s="97"/>
-      <c r="Y12" s="97"/>
-      <c r="Z12" s="97"/>
-      <c r="AA12" s="97"/>
-      <c r="AB12" s="98"/>
+      <c r="U12" s="119"/>
+      <c r="V12" s="120"/>
+      <c r="W12" s="120"/>
+      <c r="X12" s="120"/>
+      <c r="Y12" s="120"/>
+      <c r="Z12" s="120"/>
+      <c r="AA12" s="120"/>
+      <c r="AB12" s="121"/>
       <c r="AC12" s="42"/>
       <c r="AD12" s="20"/>
       <c r="AE12" s="40"/>
@@ -3234,12 +3239,12 @@
       <c r="AH12" s="20"/>
       <c r="AI12" s="20"/>
       <c r="AJ12" s="41"/>
-      <c r="AK12" s="105"/>
-      <c r="AL12" s="106"/>
-      <c r="AM12" s="106"/>
-      <c r="AN12" s="107"/>
-      <c r="AO12" s="40"/>
-      <c r="AP12" s="40"/>
+      <c r="AK12" s="92"/>
+      <c r="AL12" s="93"/>
+      <c r="AM12" s="93"/>
+      <c r="AN12" s="94"/>
+      <c r="AO12" s="20"/>
+      <c r="AP12" s="20"/>
       <c r="AQ12" s="40"/>
       <c r="AR12" s="41"/>
       <c r="AS12" s="42"/>
@@ -3250,10 +3255,10 @@
       <c r="AX12" s="40"/>
       <c r="AY12" s="40"/>
       <c r="AZ12" s="41"/>
-      <c r="BA12" s="105"/>
-      <c r="BB12" s="106"/>
-      <c r="BC12" s="106"/>
-      <c r="BD12" s="107"/>
+      <c r="BA12" s="92"/>
+      <c r="BB12" s="93"/>
+      <c r="BC12" s="93"/>
+      <c r="BD12" s="94"/>
       <c r="BE12" s="40"/>
       <c r="BF12" s="40"/>
       <c r="BG12" s="40"/>
@@ -3266,10 +3271,10 @@
       <c r="BN12" s="40"/>
       <c r="BO12" s="40"/>
       <c r="BP12" s="41"/>
-      <c r="BQ12" s="105"/>
-      <c r="BR12" s="106"/>
-      <c r="BS12" s="106"/>
-      <c r="BT12" s="107"/>
+      <c r="BQ12" s="92"/>
+      <c r="BR12" s="93"/>
+      <c r="BS12" s="93"/>
+      <c r="BT12" s="94"/>
       <c r="BU12" s="40"/>
       <c r="BV12" s="40"/>
       <c r="BW12" s="40"/>
@@ -3284,7 +3289,7 @@
       <c r="CF12" s="41"/>
     </row>
     <row r="13" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="116"/>
+      <c r="A13" s="130"/>
       <c r="B13" s="75" t="s">
         <v>30</v>
       </c>
@@ -3292,10 +3297,10 @@
         <v>23</v>
       </c>
       <c r="D13" s="25"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="89"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="112"/>
       <c r="I13" s="40"/>
       <c r="J13" s="40"/>
       <c r="K13" s="40"/>
@@ -3308,14 +3313,14 @@
       <c r="R13" s="40"/>
       <c r="S13" s="40"/>
       <c r="T13" s="41"/>
-      <c r="U13" s="96"/>
-      <c r="V13" s="97"/>
-      <c r="W13" s="97"/>
-      <c r="X13" s="97"/>
-      <c r="Y13" s="97"/>
-      <c r="Z13" s="97"/>
-      <c r="AA13" s="97"/>
-      <c r="AB13" s="98"/>
+      <c r="U13" s="119"/>
+      <c r="V13" s="120"/>
+      <c r="W13" s="120"/>
+      <c r="X13" s="120"/>
+      <c r="Y13" s="120"/>
+      <c r="Z13" s="120"/>
+      <c r="AA13" s="120"/>
+      <c r="AB13" s="121"/>
       <c r="AC13" s="42"/>
       <c r="AD13" s="40"/>
       <c r="AE13" s="20"/>
@@ -3324,10 +3329,10 @@
       <c r="AH13" s="40"/>
       <c r="AI13" s="40"/>
       <c r="AJ13" s="69"/>
-      <c r="AK13" s="105"/>
-      <c r="AL13" s="106"/>
-      <c r="AM13" s="106"/>
-      <c r="AN13" s="107"/>
+      <c r="AK13" s="92"/>
+      <c r="AL13" s="93"/>
+      <c r="AM13" s="93"/>
+      <c r="AN13" s="94"/>
       <c r="AO13" s="40"/>
       <c r="AP13" s="40"/>
       <c r="AQ13" s="40"/>
@@ -3340,10 +3345,10 @@
       <c r="AX13" s="40"/>
       <c r="AY13" s="40"/>
       <c r="AZ13" s="41"/>
-      <c r="BA13" s="105"/>
-      <c r="BB13" s="106"/>
-      <c r="BC13" s="106"/>
-      <c r="BD13" s="107"/>
+      <c r="BA13" s="92"/>
+      <c r="BB13" s="93"/>
+      <c r="BC13" s="93"/>
+      <c r="BD13" s="94"/>
       <c r="BE13" s="40"/>
       <c r="BF13" s="40"/>
       <c r="BG13" s="40"/>
@@ -3356,10 +3361,10 @@
       <c r="BN13" s="40"/>
       <c r="BO13" s="40"/>
       <c r="BP13" s="41"/>
-      <c r="BQ13" s="105"/>
-      <c r="BR13" s="106"/>
-      <c r="BS13" s="106"/>
-      <c r="BT13" s="107"/>
+      <c r="BQ13" s="92"/>
+      <c r="BR13" s="93"/>
+      <c r="BS13" s="93"/>
+      <c r="BT13" s="94"/>
       <c r="BU13" s="40"/>
       <c r="BV13" s="40"/>
       <c r="BW13" s="40"/>
@@ -3374,16 +3379,18 @@
       <c r="CF13" s="41"/>
     </row>
     <row r="14" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="117"/>
+      <c r="A14" s="131"/>
       <c r="B14" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="15" t="s">
+        <v>32</v>
+      </c>
       <c r="D14" s="25"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="89"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="111"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="112"/>
       <c r="I14" s="40"/>
       <c r="J14" s="40"/>
       <c r="K14" s="40"/>
@@ -3396,14 +3403,14 @@
       <c r="R14" s="40"/>
       <c r="S14" s="40"/>
       <c r="T14" s="41"/>
-      <c r="U14" s="96"/>
-      <c r="V14" s="97"/>
-      <c r="W14" s="97"/>
-      <c r="X14" s="97"/>
-      <c r="Y14" s="97"/>
-      <c r="Z14" s="97"/>
-      <c r="AA14" s="97"/>
-      <c r="AB14" s="98"/>
+      <c r="U14" s="119"/>
+      <c r="V14" s="120"/>
+      <c r="W14" s="120"/>
+      <c r="X14" s="120"/>
+      <c r="Y14" s="120"/>
+      <c r="Z14" s="120"/>
+      <c r="AA14" s="120"/>
+      <c r="AB14" s="121"/>
       <c r="AC14" s="42"/>
       <c r="AD14" s="40"/>
       <c r="AE14" s="40"/>
@@ -3412,13 +3419,13 @@
       <c r="AH14" s="40"/>
       <c r="AI14" s="40"/>
       <c r="AJ14" s="70"/>
-      <c r="AK14" s="105"/>
-      <c r="AL14" s="106"/>
-      <c r="AM14" s="106"/>
-      <c r="AN14" s="107"/>
+      <c r="AK14" s="92"/>
+      <c r="AL14" s="93"/>
+      <c r="AM14" s="93"/>
+      <c r="AN14" s="94"/>
       <c r="AO14" s="40"/>
       <c r="AP14" s="40"/>
-      <c r="AQ14" s="40"/>
+      <c r="AQ14" s="20"/>
       <c r="AR14" s="41"/>
       <c r="AS14" s="42"/>
       <c r="AT14" s="40"/>
@@ -3428,10 +3435,10 @@
       <c r="AX14" s="40"/>
       <c r="AY14" s="40"/>
       <c r="AZ14" s="41"/>
-      <c r="BA14" s="105"/>
-      <c r="BB14" s="106"/>
-      <c r="BC14" s="106"/>
-      <c r="BD14" s="107"/>
+      <c r="BA14" s="92"/>
+      <c r="BB14" s="93"/>
+      <c r="BC14" s="93"/>
+      <c r="BD14" s="94"/>
       <c r="BE14" s="40"/>
       <c r="BF14" s="40"/>
       <c r="BG14" s="40"/>
@@ -3444,10 +3451,10 @@
       <c r="BN14" s="40"/>
       <c r="BO14" s="40"/>
       <c r="BP14" s="41"/>
-      <c r="BQ14" s="105"/>
-      <c r="BR14" s="106"/>
-      <c r="BS14" s="106"/>
-      <c r="BT14" s="107"/>
+      <c r="BQ14" s="92"/>
+      <c r="BR14" s="93"/>
+      <c r="BS14" s="93"/>
+      <c r="BT14" s="94"/>
       <c r="BU14" s="40"/>
       <c r="BV14" s="40"/>
       <c r="BW14" s="40"/>
@@ -3462,7 +3469,7 @@
       <c r="CF14" s="41"/>
     </row>
     <row r="15" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="111" t="s">
+      <c r="A15" s="125" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="73" t="s">
@@ -3470,10 +3477,10 @@
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="25"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="89"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="111"/>
+      <c r="H15" s="112"/>
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
       <c r="K15" s="43"/>
@@ -3486,14 +3493,14 @@
       <c r="R15" s="43"/>
       <c r="S15" s="43"/>
       <c r="T15" s="44"/>
-      <c r="U15" s="96"/>
-      <c r="V15" s="97"/>
-      <c r="W15" s="97"/>
-      <c r="X15" s="97"/>
-      <c r="Y15" s="97"/>
-      <c r="Z15" s="97"/>
-      <c r="AA15" s="97"/>
-      <c r="AB15" s="98"/>
+      <c r="U15" s="119"/>
+      <c r="V15" s="120"/>
+      <c r="W15" s="120"/>
+      <c r="X15" s="120"/>
+      <c r="Y15" s="120"/>
+      <c r="Z15" s="120"/>
+      <c r="AA15" s="120"/>
+      <c r="AB15" s="121"/>
       <c r="AC15" s="45"/>
       <c r="AD15" s="43"/>
       <c r="AE15" s="43"/>
@@ -3502,13 +3509,13 @@
       <c r="AH15" s="43"/>
       <c r="AI15" s="43"/>
       <c r="AJ15" s="44"/>
-      <c r="AK15" s="105"/>
-      <c r="AL15" s="106"/>
-      <c r="AM15" s="106"/>
-      <c r="AN15" s="107"/>
-      <c r="AO15" s="20"/>
-      <c r="AP15" s="20"/>
-      <c r="AQ15" s="20"/>
+      <c r="AK15" s="92"/>
+      <c r="AL15" s="93"/>
+      <c r="AM15" s="93"/>
+      <c r="AN15" s="94"/>
+      <c r="AO15" s="43"/>
+      <c r="AP15" s="43"/>
+      <c r="AQ15" s="43"/>
       <c r="AR15" s="21"/>
       <c r="AS15" s="22"/>
       <c r="AT15" s="20"/>
@@ -3518,10 +3525,10 @@
       <c r="AX15" s="20"/>
       <c r="AY15" s="20"/>
       <c r="AZ15" s="44"/>
-      <c r="BA15" s="105"/>
-      <c r="BB15" s="106"/>
-      <c r="BC15" s="106"/>
-      <c r="BD15" s="107"/>
+      <c r="BA15" s="92"/>
+      <c r="BB15" s="93"/>
+      <c r="BC15" s="93"/>
+      <c r="BD15" s="94"/>
       <c r="BE15" s="43"/>
       <c r="BF15" s="43"/>
       <c r="BG15" s="43"/>
@@ -3534,10 +3541,10 @@
       <c r="BN15" s="43"/>
       <c r="BO15" s="43"/>
       <c r="BP15" s="44"/>
-      <c r="BQ15" s="105"/>
-      <c r="BR15" s="106"/>
-      <c r="BS15" s="106"/>
-      <c r="BT15" s="107"/>
+      <c r="BQ15" s="92"/>
+      <c r="BR15" s="93"/>
+      <c r="BS15" s="93"/>
+      <c r="BT15" s="94"/>
       <c r="BU15" s="43"/>
       <c r="BV15" s="43"/>
       <c r="BW15" s="43"/>
@@ -3552,16 +3559,16 @@
       <c r="CF15" s="44"/>
     </row>
     <row r="16" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="112"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="80" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="25"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="88"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="89"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="111"/>
+      <c r="G16" s="111"/>
+      <c r="H16" s="112"/>
       <c r="I16" s="43"/>
       <c r="J16" s="43"/>
       <c r="K16" s="43"/>
@@ -3574,14 +3581,14 @@
       <c r="R16" s="43"/>
       <c r="S16" s="43"/>
       <c r="T16" s="44"/>
-      <c r="U16" s="96"/>
-      <c r="V16" s="97"/>
-      <c r="W16" s="97"/>
-      <c r="X16" s="97"/>
-      <c r="Y16" s="97"/>
-      <c r="Z16" s="97"/>
-      <c r="AA16" s="97"/>
-      <c r="AB16" s="98"/>
+      <c r="U16" s="119"/>
+      <c r="V16" s="120"/>
+      <c r="W16" s="120"/>
+      <c r="X16" s="120"/>
+      <c r="Y16" s="120"/>
+      <c r="Z16" s="120"/>
+      <c r="AA16" s="120"/>
+      <c r="AB16" s="121"/>
       <c r="AC16" s="45"/>
       <c r="AD16" s="43"/>
       <c r="AE16" s="43"/>
@@ -3590,10 +3597,10 @@
       <c r="AH16" s="43"/>
       <c r="AI16" s="43"/>
       <c r="AJ16" s="44"/>
-      <c r="AK16" s="105"/>
-      <c r="AL16" s="106"/>
-      <c r="AM16" s="106"/>
-      <c r="AN16" s="107"/>
+      <c r="AK16" s="92"/>
+      <c r="AL16" s="93"/>
+      <c r="AM16" s="93"/>
+      <c r="AN16" s="94"/>
       <c r="AO16" s="43"/>
       <c r="AP16" s="43"/>
       <c r="AQ16" s="43"/>
@@ -3606,10 +3613,10 @@
       <c r="AX16" s="43"/>
       <c r="AY16" s="43"/>
       <c r="AZ16" s="70"/>
-      <c r="BA16" s="105"/>
-      <c r="BB16" s="106"/>
-      <c r="BC16" s="106"/>
-      <c r="BD16" s="107"/>
+      <c r="BA16" s="92"/>
+      <c r="BB16" s="93"/>
+      <c r="BC16" s="93"/>
+      <c r="BD16" s="94"/>
       <c r="BE16" s="43"/>
       <c r="BF16" s="43"/>
       <c r="BG16" s="43"/>
@@ -3622,10 +3629,10 @@
       <c r="BN16" s="43"/>
       <c r="BO16" s="43"/>
       <c r="BP16" s="44"/>
-      <c r="BQ16" s="105"/>
-      <c r="BR16" s="106"/>
-      <c r="BS16" s="106"/>
-      <c r="BT16" s="107"/>
+      <c r="BQ16" s="92"/>
+      <c r="BR16" s="93"/>
+      <c r="BS16" s="93"/>
+      <c r="BT16" s="94"/>
       <c r="BU16" s="43"/>
       <c r="BV16" s="43"/>
       <c r="BW16" s="43"/>
@@ -3640,7 +3647,7 @@
       <c r="CF16" s="44"/>
     </row>
     <row r="17" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="113" t="s">
+      <c r="A17" s="127" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="72" t="s">
@@ -3648,10 +3655,10 @@
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="88"/>
-      <c r="H17" s="89"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="111"/>
+      <c r="G17" s="111"/>
+      <c r="H17" s="112"/>
       <c r="I17" s="46"/>
       <c r="J17" s="46"/>
       <c r="K17" s="46"/>
@@ -3664,14 +3671,14 @@
       <c r="R17" s="46"/>
       <c r="S17" s="46"/>
       <c r="T17" s="47"/>
-      <c r="U17" s="96"/>
-      <c r="V17" s="97"/>
-      <c r="W17" s="97"/>
-      <c r="X17" s="97"/>
-      <c r="Y17" s="97"/>
-      <c r="Z17" s="97"/>
-      <c r="AA17" s="97"/>
-      <c r="AB17" s="98"/>
+      <c r="U17" s="119"/>
+      <c r="V17" s="120"/>
+      <c r="W17" s="120"/>
+      <c r="X17" s="120"/>
+      <c r="Y17" s="120"/>
+      <c r="Z17" s="120"/>
+      <c r="AA17" s="120"/>
+      <c r="AB17" s="121"/>
       <c r="AC17" s="48"/>
       <c r="AD17" s="46"/>
       <c r="AE17" s="46"/>
@@ -3680,10 +3687,10 @@
       <c r="AH17" s="46"/>
       <c r="AI17" s="46"/>
       <c r="AJ17" s="47"/>
-      <c r="AK17" s="105"/>
-      <c r="AL17" s="106"/>
-      <c r="AM17" s="106"/>
-      <c r="AN17" s="107"/>
+      <c r="AK17" s="92"/>
+      <c r="AL17" s="93"/>
+      <c r="AM17" s="93"/>
+      <c r="AN17" s="94"/>
       <c r="AO17" s="46"/>
       <c r="AP17" s="46"/>
       <c r="AQ17" s="46"/>
@@ -3696,10 +3703,10 @@
       <c r="AX17" s="46"/>
       <c r="AY17" s="46"/>
       <c r="AZ17" s="47"/>
-      <c r="BA17" s="105"/>
-      <c r="BB17" s="106"/>
-      <c r="BC17" s="106"/>
-      <c r="BD17" s="107"/>
+      <c r="BA17" s="92"/>
+      <c r="BB17" s="93"/>
+      <c r="BC17" s="93"/>
+      <c r="BD17" s="94"/>
       <c r="BE17" s="20"/>
       <c r="BF17" s="20"/>
       <c r="BG17" s="20"/>
@@ -3712,10 +3719,10 @@
       <c r="BN17" s="20"/>
       <c r="BO17" s="20"/>
       <c r="BP17" s="47"/>
-      <c r="BQ17" s="105"/>
-      <c r="BR17" s="106"/>
-      <c r="BS17" s="106"/>
-      <c r="BT17" s="107"/>
+      <c r="BQ17" s="92"/>
+      <c r="BR17" s="93"/>
+      <c r="BS17" s="93"/>
+      <c r="BT17" s="94"/>
       <c r="BU17" s="46"/>
       <c r="BV17" s="46"/>
       <c r="BW17" s="46"/>
@@ -3730,16 +3737,16 @@
       <c r="CF17" s="47"/>
     </row>
     <row r="18" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="114"/>
+      <c r="A18" s="128"/>
       <c r="B18" s="79" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="25"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="88"/>
-      <c r="G18" s="88"/>
-      <c r="H18" s="89"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="112"/>
       <c r="I18" s="46"/>
       <c r="J18" s="46"/>
       <c r="K18" s="46"/>
@@ -3752,14 +3759,14 @@
       <c r="R18" s="46"/>
       <c r="S18" s="46"/>
       <c r="T18" s="47"/>
-      <c r="U18" s="96"/>
-      <c r="V18" s="97"/>
-      <c r="W18" s="97"/>
-      <c r="X18" s="97"/>
-      <c r="Y18" s="97"/>
-      <c r="Z18" s="97"/>
-      <c r="AA18" s="97"/>
-      <c r="AB18" s="98"/>
+      <c r="U18" s="119"/>
+      <c r="V18" s="120"/>
+      <c r="W18" s="120"/>
+      <c r="X18" s="120"/>
+      <c r="Y18" s="120"/>
+      <c r="Z18" s="120"/>
+      <c r="AA18" s="120"/>
+      <c r="AB18" s="121"/>
       <c r="AC18" s="48"/>
       <c r="AD18" s="46"/>
       <c r="AE18" s="46"/>
@@ -3768,10 +3775,10 @@
       <c r="AH18" s="46"/>
       <c r="AI18" s="46"/>
       <c r="AJ18" s="47"/>
-      <c r="AK18" s="105"/>
-      <c r="AL18" s="106"/>
-      <c r="AM18" s="106"/>
-      <c r="AN18" s="107"/>
+      <c r="AK18" s="92"/>
+      <c r="AL18" s="93"/>
+      <c r="AM18" s="93"/>
+      <c r="AN18" s="94"/>
       <c r="AO18" s="46"/>
       <c r="AP18" s="46"/>
       <c r="AQ18" s="46"/>
@@ -3784,10 +3791,10 @@
       <c r="AX18" s="46"/>
       <c r="AY18" s="46"/>
       <c r="AZ18" s="47"/>
-      <c r="BA18" s="105"/>
-      <c r="BB18" s="106"/>
-      <c r="BC18" s="106"/>
-      <c r="BD18" s="107"/>
+      <c r="BA18" s="92"/>
+      <c r="BB18" s="93"/>
+      <c r="BC18" s="93"/>
+      <c r="BD18" s="94"/>
       <c r="BE18" s="46"/>
       <c r="BF18" s="46"/>
       <c r="BG18" s="46"/>
@@ -3800,10 +3807,10 @@
       <c r="BN18" s="46"/>
       <c r="BO18" s="46"/>
       <c r="BP18" s="21"/>
-      <c r="BQ18" s="105"/>
-      <c r="BR18" s="106"/>
-      <c r="BS18" s="106"/>
-      <c r="BT18" s="107"/>
+      <c r="BQ18" s="92"/>
+      <c r="BR18" s="93"/>
+      <c r="BS18" s="93"/>
+      <c r="BT18" s="94"/>
       <c r="BU18" s="46"/>
       <c r="BV18" s="46"/>
       <c r="BW18" s="46"/>
@@ -3818,7 +3825,7 @@
       <c r="CF18" s="47"/>
     </row>
     <row r="19" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="118" t="s">
+      <c r="A19" s="132" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="77" t="s">
@@ -3826,10 +3833,10 @@
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="25"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="88"/>
-      <c r="G19" s="88"/>
-      <c r="H19" s="89"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111"/>
+      <c r="H19" s="112"/>
       <c r="I19" s="49"/>
       <c r="J19" s="49"/>
       <c r="K19" s="49"/>
@@ -3842,14 +3849,14 @@
       <c r="R19" s="49"/>
       <c r="S19" s="49"/>
       <c r="T19" s="50"/>
-      <c r="U19" s="96"/>
-      <c r="V19" s="97"/>
-      <c r="W19" s="97"/>
-      <c r="X19" s="97"/>
-      <c r="Y19" s="97"/>
-      <c r="Z19" s="97"/>
-      <c r="AA19" s="97"/>
-      <c r="AB19" s="98"/>
+      <c r="U19" s="119"/>
+      <c r="V19" s="120"/>
+      <c r="W19" s="120"/>
+      <c r="X19" s="120"/>
+      <c r="Y19" s="120"/>
+      <c r="Z19" s="120"/>
+      <c r="AA19" s="120"/>
+      <c r="AB19" s="121"/>
       <c r="AC19" s="51"/>
       <c r="AD19" s="49"/>
       <c r="AE19" s="49"/>
@@ -3858,10 +3865,10 @@
       <c r="AH19" s="49"/>
       <c r="AI19" s="49"/>
       <c r="AJ19" s="50"/>
-      <c r="AK19" s="105"/>
-      <c r="AL19" s="106"/>
-      <c r="AM19" s="106"/>
-      <c r="AN19" s="107"/>
+      <c r="AK19" s="92"/>
+      <c r="AL19" s="93"/>
+      <c r="AM19" s="93"/>
+      <c r="AN19" s="94"/>
       <c r="AO19" s="49"/>
       <c r="AP19" s="49"/>
       <c r="AQ19" s="49"/>
@@ -3874,10 +3881,10 @@
       <c r="AX19" s="49"/>
       <c r="AY19" s="49"/>
       <c r="AZ19" s="50"/>
-      <c r="BA19" s="105"/>
-      <c r="BB19" s="106"/>
-      <c r="BC19" s="106"/>
-      <c r="BD19" s="107"/>
+      <c r="BA19" s="92"/>
+      <c r="BB19" s="93"/>
+      <c r="BC19" s="93"/>
+      <c r="BD19" s="94"/>
       <c r="BE19" s="49"/>
       <c r="BF19" s="49"/>
       <c r="BG19" s="49"/>
@@ -3890,10 +3897,10 @@
       <c r="BN19" s="49"/>
       <c r="BO19" s="49"/>
       <c r="BP19" s="50"/>
-      <c r="BQ19" s="105"/>
-      <c r="BR19" s="106"/>
-      <c r="BS19" s="106"/>
-      <c r="BT19" s="107"/>
+      <c r="BQ19" s="92"/>
+      <c r="BR19" s="93"/>
+      <c r="BS19" s="93"/>
+      <c r="BT19" s="94"/>
       <c r="BU19" s="20"/>
       <c r="BV19" s="20"/>
       <c r="BW19" s="20"/>
@@ -3908,16 +3915,16 @@
       <c r="CF19" s="50"/>
     </row>
     <row r="20" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="119"/>
+      <c r="A20" s="133"/>
       <c r="B20" s="81" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="25"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="89"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="111"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="112"/>
       <c r="I20" s="65"/>
       <c r="J20" s="65"/>
       <c r="K20" s="65"/>
@@ -3930,14 +3937,14 @@
       <c r="R20" s="65"/>
       <c r="S20" s="65"/>
       <c r="T20" s="66"/>
-      <c r="U20" s="96"/>
-      <c r="V20" s="97"/>
-      <c r="W20" s="97"/>
-      <c r="X20" s="97"/>
-      <c r="Y20" s="97"/>
-      <c r="Z20" s="97"/>
-      <c r="AA20" s="97"/>
-      <c r="AB20" s="98"/>
+      <c r="U20" s="119"/>
+      <c r="V20" s="120"/>
+      <c r="W20" s="120"/>
+      <c r="X20" s="120"/>
+      <c r="Y20" s="120"/>
+      <c r="Z20" s="120"/>
+      <c r="AA20" s="120"/>
+      <c r="AB20" s="121"/>
       <c r="AC20" s="67"/>
       <c r="AD20" s="65"/>
       <c r="AE20" s="65"/>
@@ -3946,10 +3953,10 @@
       <c r="AH20" s="65"/>
       <c r="AI20" s="65"/>
       <c r="AJ20" s="66"/>
-      <c r="AK20" s="105"/>
-      <c r="AL20" s="106"/>
-      <c r="AM20" s="106"/>
-      <c r="AN20" s="107"/>
+      <c r="AK20" s="92"/>
+      <c r="AL20" s="93"/>
+      <c r="AM20" s="93"/>
+      <c r="AN20" s="94"/>
       <c r="AO20" s="65"/>
       <c r="AP20" s="65"/>
       <c r="AQ20" s="65"/>
@@ -3962,10 +3969,10 @@
       <c r="AX20" s="65"/>
       <c r="AY20" s="65"/>
       <c r="AZ20" s="66"/>
-      <c r="BA20" s="105"/>
-      <c r="BB20" s="106"/>
-      <c r="BC20" s="106"/>
-      <c r="BD20" s="107"/>
+      <c r="BA20" s="92"/>
+      <c r="BB20" s="93"/>
+      <c r="BC20" s="93"/>
+      <c r="BD20" s="94"/>
       <c r="BE20" s="65"/>
       <c r="BF20" s="65"/>
       <c r="BG20" s="65"/>
@@ -3978,10 +3985,10 @@
       <c r="BN20" s="65"/>
       <c r="BO20" s="65"/>
       <c r="BP20" s="66"/>
-      <c r="BQ20" s="105"/>
-      <c r="BR20" s="106"/>
-      <c r="BS20" s="106"/>
-      <c r="BT20" s="107"/>
+      <c r="BQ20" s="92"/>
+      <c r="BR20" s="93"/>
+      <c r="BS20" s="93"/>
+      <c r="BT20" s="94"/>
       <c r="BU20" s="65"/>
       <c r="BV20" s="65"/>
       <c r="BW20" s="65"/>
@@ -4004,10 +4011,10 @@
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="25"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="88"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="89"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="111"/>
+      <c r="H21" s="112"/>
       <c r="I21" s="53"/>
       <c r="J21" s="53"/>
       <c r="K21" s="53"/>
@@ -4020,14 +4027,14 @@
       <c r="R21" s="53"/>
       <c r="S21" s="53"/>
       <c r="T21" s="54"/>
-      <c r="U21" s="96"/>
-      <c r="V21" s="97"/>
-      <c r="W21" s="97"/>
-      <c r="X21" s="97"/>
-      <c r="Y21" s="97"/>
-      <c r="Z21" s="97"/>
-      <c r="AA21" s="97"/>
-      <c r="AB21" s="98"/>
+      <c r="U21" s="119"/>
+      <c r="V21" s="120"/>
+      <c r="W21" s="120"/>
+      <c r="X21" s="120"/>
+      <c r="Y21" s="120"/>
+      <c r="Z21" s="120"/>
+      <c r="AA21" s="120"/>
+      <c r="AB21" s="121"/>
       <c r="AC21" s="55"/>
       <c r="AD21" s="53"/>
       <c r="AE21" s="53"/>
@@ -4036,10 +4043,10 @@
       <c r="AH21" s="53"/>
       <c r="AI21" s="53"/>
       <c r="AJ21" s="54"/>
-      <c r="AK21" s="105"/>
-      <c r="AL21" s="106"/>
-      <c r="AM21" s="106"/>
-      <c r="AN21" s="107"/>
+      <c r="AK21" s="92"/>
+      <c r="AL21" s="93"/>
+      <c r="AM21" s="93"/>
+      <c r="AN21" s="94"/>
       <c r="AO21" s="53"/>
       <c r="AP21" s="53"/>
       <c r="AQ21" s="53"/>
@@ -4052,10 +4059,10 @@
       <c r="AX21" s="53"/>
       <c r="AY21" s="53"/>
       <c r="AZ21" s="54"/>
-      <c r="BA21" s="105"/>
-      <c r="BB21" s="106"/>
-      <c r="BC21" s="106"/>
-      <c r="BD21" s="107"/>
+      <c r="BA21" s="92"/>
+      <c r="BB21" s="93"/>
+      <c r="BC21" s="93"/>
+      <c r="BD21" s="94"/>
       <c r="BE21" s="53"/>
       <c r="BF21" s="53"/>
       <c r="BG21" s="53"/>
@@ -4068,10 +4075,10 @@
       <c r="BN21" s="53"/>
       <c r="BO21" s="53"/>
       <c r="BP21" s="54"/>
-      <c r="BQ21" s="105"/>
-      <c r="BR21" s="106"/>
-      <c r="BS21" s="106"/>
-      <c r="BT21" s="107"/>
+      <c r="BQ21" s="92"/>
+      <c r="BR21" s="93"/>
+      <c r="BS21" s="93"/>
+      <c r="BT21" s="94"/>
       <c r="BU21" s="53"/>
       <c r="BV21" s="53"/>
       <c r="BW21" s="53"/>
@@ -4086,7 +4093,7 @@
       <c r="CF21" s="23"/>
     </row>
     <row r="22" spans="1:84" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="105" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="57" t="s">
@@ -4095,10 +4102,10 @@
       <c r="C22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="87"/>
-      <c r="F22" s="88"/>
-      <c r="G22" s="88"/>
-      <c r="H22" s="89"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="111"/>
+      <c r="G22" s="111"/>
+      <c r="H22" s="112"/>
       <c r="I22" s="59"/>
       <c r="J22" s="59"/>
       <c r="K22" s="59"/>
@@ -4111,83 +4118,83 @@
       <c r="R22" s="59"/>
       <c r="S22" s="59"/>
       <c r="T22" s="60"/>
-      <c r="U22" s="96"/>
-      <c r="V22" s="97"/>
-      <c r="W22" s="97"/>
-      <c r="X22" s="97"/>
-      <c r="Y22" s="97"/>
-      <c r="Z22" s="97"/>
-      <c r="AA22" s="97"/>
-      <c r="AB22" s="98"/>
+      <c r="U22" s="119"/>
+      <c r="V22" s="120"/>
+      <c r="W22" s="120"/>
+      <c r="X22" s="120"/>
+      <c r="Y22" s="120"/>
+      <c r="Z22" s="120"/>
+      <c r="AA22" s="120"/>
+      <c r="AB22" s="121"/>
       <c r="AC22" s="58"/>
       <c r="AD22" s="59"/>
       <c r="AE22" s="59"/>
       <c r="AF22" s="59"/>
       <c r="AG22" s="59"/>
       <c r="AH22" s="59"/>
-      <c r="AI22" s="135"/>
-      <c r="AJ22" s="136"/>
-      <c r="AK22" s="105"/>
-      <c r="AL22" s="106"/>
-      <c r="AM22" s="106"/>
-      <c r="AN22" s="107"/>
-      <c r="AO22" s="59"/>
-      <c r="AP22" s="59"/>
-      <c r="AQ22" s="59"/>
-      <c r="AR22" s="136"/>
+      <c r="AI22" s="82"/>
+      <c r="AJ22" s="83"/>
+      <c r="AK22" s="92"/>
+      <c r="AL22" s="93"/>
+      <c r="AM22" s="93"/>
+      <c r="AN22" s="94"/>
+      <c r="AO22" s="82"/>
+      <c r="AP22" s="82"/>
+      <c r="AQ22" s="82"/>
+      <c r="AR22" s="83"/>
       <c r="AS22" s="58"/>
       <c r="AT22" s="59"/>
       <c r="AU22" s="59"/>
       <c r="AV22" s="59"/>
       <c r="AW22" s="59"/>
-      <c r="AX22" s="135"/>
-      <c r="AY22" s="135"/>
-      <c r="AZ22" s="136"/>
-      <c r="BA22" s="105"/>
-      <c r="BB22" s="106"/>
-      <c r="BC22" s="106"/>
-      <c r="BD22" s="107"/>
-      <c r="BE22" s="59"/>
-      <c r="BF22" s="59"/>
+      <c r="AX22" s="59"/>
+      <c r="AY22" s="59"/>
+      <c r="AZ22" s="60"/>
+      <c r="BA22" s="92"/>
+      <c r="BB22" s="93"/>
+      <c r="BC22" s="93"/>
+      <c r="BD22" s="94"/>
+      <c r="BE22" s="82"/>
+      <c r="BF22" s="82"/>
       <c r="BG22" s="59"/>
-      <c r="BH22" s="136"/>
+      <c r="BH22" s="60"/>
       <c r="BI22" s="58"/>
       <c r="BJ22" s="59"/>
       <c r="BK22" s="59"/>
       <c r="BL22" s="59"/>
       <c r="BM22" s="59"/>
-      <c r="BN22" s="135"/>
-      <c r="BO22" s="135"/>
-      <c r="BP22" s="136"/>
-      <c r="BQ22" s="105"/>
-      <c r="BR22" s="106"/>
-      <c r="BS22" s="106"/>
-      <c r="BT22" s="107"/>
+      <c r="BN22" s="82"/>
+      <c r="BO22" s="82"/>
+      <c r="BP22" s="83"/>
+      <c r="BQ22" s="92"/>
+      <c r="BR22" s="93"/>
+      <c r="BS22" s="93"/>
+      <c r="BT22" s="94"/>
       <c r="BU22" s="59"/>
       <c r="BV22" s="59"/>
       <c r="BW22" s="59"/>
-      <c r="BX22" s="136"/>
+      <c r="BX22" s="83"/>
       <c r="BY22" s="58"/>
       <c r="BZ22" s="59"/>
       <c r="CA22" s="59"/>
-      <c r="CB22" s="135"/>
-      <c r="CC22" s="135"/>
-      <c r="CD22" s="135"/>
-      <c r="CE22" s="135"/>
+      <c r="CB22" s="82"/>
+      <c r="CC22" s="82"/>
+      <c r="CD22" s="82"/>
+      <c r="CE22" s="82"/>
       <c r="CF22" s="60"/>
     </row>
     <row r="23" spans="1:84" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
+      <c r="A23" s="106"/>
       <c r="B23" s="56" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="90"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="92"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="114"/>
+      <c r="G23" s="114"/>
+      <c r="H23" s="115"/>
       <c r="I23" s="64"/>
       <c r="J23" s="64"/>
       <c r="K23" s="62"/>
@@ -4200,14 +4207,14 @@
       <c r="R23" s="62"/>
       <c r="S23" s="62"/>
       <c r="T23" s="63"/>
-      <c r="U23" s="99"/>
-      <c r="V23" s="100"/>
-      <c r="W23" s="100"/>
-      <c r="X23" s="100"/>
-      <c r="Y23" s="100"/>
-      <c r="Z23" s="100"/>
-      <c r="AA23" s="100"/>
-      <c r="AB23" s="101"/>
+      <c r="U23" s="122"/>
+      <c r="V23" s="123"/>
+      <c r="W23" s="123"/>
+      <c r="X23" s="123"/>
+      <c r="Y23" s="123"/>
+      <c r="Z23" s="123"/>
+      <c r="AA23" s="123"/>
+      <c r="AB23" s="124"/>
       <c r="AC23" s="61"/>
       <c r="AD23" s="62"/>
       <c r="AE23" s="62"/>
@@ -4216,10 +4223,10 @@
       <c r="AH23" s="62"/>
       <c r="AI23" s="62"/>
       <c r="AJ23" s="63"/>
-      <c r="AK23" s="108"/>
-      <c r="AL23" s="109"/>
-      <c r="AM23" s="109"/>
-      <c r="AN23" s="110"/>
+      <c r="AK23" s="95"/>
+      <c r="AL23" s="96"/>
+      <c r="AM23" s="96"/>
+      <c r="AN23" s="97"/>
       <c r="AO23" s="62"/>
       <c r="AP23" s="62"/>
       <c r="AQ23" s="62"/>
@@ -4232,10 +4239,10 @@
       <c r="AX23" s="62"/>
       <c r="AY23" s="62"/>
       <c r="AZ23" s="63"/>
-      <c r="BA23" s="108"/>
-      <c r="BB23" s="109"/>
-      <c r="BC23" s="109"/>
-      <c r="BD23" s="110"/>
+      <c r="BA23" s="95"/>
+      <c r="BB23" s="96"/>
+      <c r="BC23" s="96"/>
+      <c r="BD23" s="97"/>
       <c r="BE23" s="62"/>
       <c r="BF23" s="62"/>
       <c r="BG23" s="62"/>
@@ -4248,10 +4255,10 @@
       <c r="BN23" s="62"/>
       <c r="BO23" s="62"/>
       <c r="BP23" s="63"/>
-      <c r="BQ23" s="108"/>
-      <c r="BR23" s="109"/>
-      <c r="BS23" s="109"/>
-      <c r="BT23" s="110"/>
+      <c r="BQ23" s="95"/>
+      <c r="BR23" s="96"/>
+      <c r="BS23" s="96"/>
+      <c r="BT23" s="97"/>
       <c r="BU23" s="62"/>
       <c r="BV23" s="62"/>
       <c r="BW23" s="62"/>
@@ -4259,19 +4266,26 @@
       <c r="BY23" s="61"/>
       <c r="BZ23" s="62"/>
       <c r="CA23" s="62"/>
-      <c r="CB23" s="137"/>
-      <c r="CC23" s="137"/>
-      <c r="CD23" s="137"/>
-      <c r="CE23" s="137"/>
+      <c r="CB23" s="84"/>
+      <c r="CC23" s="84"/>
+      <c r="CD23" s="84"/>
+      <c r="CE23" s="84"/>
       <c r="CF23" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="U4:X4"/>
-    <mergeCell ref="Y4:AB4"/>
-    <mergeCell ref="BA6:BD23"/>
-    <mergeCell ref="BQ6:BT23"/>
+    <mergeCell ref="BU4:BX4"/>
+    <mergeCell ref="BQ4:BT4"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="E6:H23"/>
+    <mergeCell ref="U6:AB23"/>
+    <mergeCell ref="AK6:AN23"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
     <mergeCell ref="E2:AR3"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -4288,22 +4302,15 @@
     <mergeCell ref="AW4:AZ4"/>
     <mergeCell ref="BY4:CB4"/>
     <mergeCell ref="CC4:CF4"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="U4:X4"/>
+    <mergeCell ref="Y4:AB4"/>
+    <mergeCell ref="BA6:BD23"/>
+    <mergeCell ref="BQ6:BT23"/>
     <mergeCell ref="BA4:BD4"/>
     <mergeCell ref="BE4:BH4"/>
     <mergeCell ref="BI4:BL4"/>
     <mergeCell ref="BM4:BP4"/>
-    <mergeCell ref="BU4:BX4"/>
-    <mergeCell ref="BQ4:BT4"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="E6:H23"/>
-    <mergeCell ref="U6:AB23"/>
-    <mergeCell ref="AK6:AN23"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A9:A11"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="C6:C23">
@@ -4545,15 +4552,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
@@ -4562,6 +4560,15 @@
     <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4584,14 +4591,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F2702F0-3EB0-496B-8166-A9BB237AECA6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4602,4 +4601,12 @@
     <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{762EB85F-E28B-44CA-8330-7878EE38D3E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
module perso + planning
</commit_message>
<xml_diff>
--- a/documentation/3_2_PlanningJeudiVendredi.xlsx
+++ b/documentation/3_2_PlanningJeudiVendredi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/theo_pasquier_studentfr_ch/Documents/3eme année/306/projet/306-G1-Piloter_un_robot_phidget_a_distance/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="657" documentId="8_{3242CAA9-CE1B-4AB7-A89C-0F9BBFF89D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE4BA11E-9A13-46C1-A3DB-5AB0E59D0E07}"/>
+  <xr:revisionPtr revIDLastSave="660" documentId="8_{3242CAA9-CE1B-4AB7-A89C-0F9BBFF89D43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB4B5D71-95EF-4608-8C94-FE808DAD7275}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>Journée culturelle</t>
   </si>
   <si>
-    <t>Pasquier Théo</t>
-  </si>
-  <si>
     <t>Introduction</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>Sprint review</t>
+  </si>
+  <si>
+    <t>Pasquier Théo, Pires Donose Andrei &amp; Müller Luuk</t>
   </si>
 </sst>
 </file>
@@ -1403,12 +1403,12 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>771524</xdr:colOff>
+      <xdr:colOff>771523</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>76</xdr:col>
+      <xdr:col>80</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -1426,8 +1426,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5076824" y="1504950"/>
-          <a:ext cx="10734676" cy="3257550"/>
+          <a:off x="5076823" y="1504950"/>
+          <a:ext cx="11306177" cy="3257550"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2052,7 +2052,7 @@
       <pane xSplit="4" ySplit="5" topLeftCell="E9" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="Y27" sqref="Y27"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2068,7 +2068,7 @@
   <sheetData>
     <row r="1" spans="1:84" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="104" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="104"/>
       <c r="C1" s="12"/>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="2" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="105" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B2" s="106"/>
       <c r="C2" s="13"/>
@@ -2668,17 +2668,17 @@
     </row>
     <row r="6" spans="1:84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="138" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>10</v>
-      </c>
       <c r="C6" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="111" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="112"/>
       <c r="G6" s="112"/>
@@ -2714,7 +2714,7 @@
       <c r="AI6" s="30"/>
       <c r="AJ6" s="31"/>
       <c r="AK6" s="89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AL6" s="90"/>
       <c r="AM6" s="90"/>
@@ -2732,7 +2732,7 @@
       <c r="AY6" s="30"/>
       <c r="AZ6" s="31"/>
       <c r="BA6" s="89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BB6" s="90"/>
       <c r="BC6" s="90"/>
@@ -2750,7 +2750,7 @@
       <c r="BO6" s="30"/>
       <c r="BP6" s="31"/>
       <c r="BQ6" s="89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BR6" s="90"/>
       <c r="BS6" s="90"/>
@@ -2771,10 +2771,10 @@
     <row r="7" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A7" s="138"/>
       <c r="B7" s="28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="114"/>
@@ -2861,10 +2861,10 @@
     <row r="8" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A8" s="138"/>
       <c r="B8" s="29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="114"/>
@@ -2950,13 +2950,13 @@
     </row>
     <row r="9" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A9" s="139" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>14</v>
-      </c>
       <c r="C9" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="114"/>
@@ -3043,10 +3043,10 @@
     <row r="10" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A10" s="140"/>
       <c r="B10" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="114"/>
@@ -3133,10 +3133,10 @@
     <row r="11" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A11" s="141"/>
       <c r="B11" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="114"/>
@@ -3222,13 +3222,13 @@
     </row>
     <row r="12" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="133" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="74" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="114"/>
@@ -3315,10 +3315,10 @@
     <row r="13" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="134"/>
       <c r="B13" s="75" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="114"/>
@@ -3405,10 +3405,10 @@
     <row r="14" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="135"/>
       <c r="B14" s="78" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="114"/>
@@ -3494,13 +3494,13 @@
     </row>
     <row r="15" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="129" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="114"/>
@@ -3587,10 +3587,10 @@
     <row r="16" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="130"/>
       <c r="B16" s="80" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="114"/>
@@ -3676,13 +3676,13 @@
     </row>
     <row r="17" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="131" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="114"/>
@@ -3769,10 +3769,10 @@
     <row r="18" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="132"/>
       <c r="B18" s="79" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="114"/>
@@ -3858,13 +3858,13 @@
     </row>
     <row r="19" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="136" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="77" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="114"/>
@@ -3951,7 +3951,7 @@
     <row r="20" spans="1:84" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="137"/>
       <c r="B20" s="81" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="25"/>
@@ -4038,10 +4038,10 @@
     </row>
     <row r="21" spans="1:84" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="76" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="25"/>
@@ -4128,13 +4128,13 @@
     </row>
     <row r="22" spans="1:84" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="109" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E22" s="114"/>
       <c r="F22" s="115"/>
@@ -4220,10 +4220,10 @@
     <row r="23" spans="1:84" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="110"/>
       <c r="B23" s="56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23" s="117"/>
       <c r="F23" s="118"/>

</xml_diff>